<commit_message>
Rubric and example revisions
</commit_message>
<xml_diff>
--- a/Labs/Lab03/CS133JS_Lab03_Rubric.xlsx
+++ b/Labs/Lab03/CS133JS_Lab03_Rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS133JS-CourseMaterials/Labs/Lab03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33596D5-B213-8249-AA5E-8C7C131B983A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95F548B-A2F9-B34E-9AC8-E6D4D0248CF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10180" yWindow="500" windowWidth="15420" windowHeight="14540" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="6560" yWindow="500" windowWidth="15360" windowHeight="14540" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Group A" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Criteria</t>
   </si>
@@ -51,15 +51,9 @@
     <t>Review of your code with completed "Prod." column</t>
   </si>
   <si>
-    <t>Web app 1 functionality</t>
-  </si>
-  <si>
     <t xml:space="preserve">   I/O in the HTML file</t>
   </si>
   <si>
-    <t>Web app 2 functionality</t>
-  </si>
-  <si>
     <t xml:space="preserve">   Code in the .js file</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>Selection exercises</t>
   </si>
   <si>
-    <t>Web app 3 functionality</t>
-  </si>
-  <si>
     <t>Web Page I</t>
   </si>
   <si>
@@ -121,13 +112,43 @@
   </si>
   <si>
     <t>Not best selection statement</t>
+  </si>
+  <si>
+    <t>Kindergarten test data:</t>
+  </si>
+  <si>
+    <t>age 5, bDay before : yes</t>
+  </si>
+  <si>
+    <t>age 5, bDay after : too young</t>
+  </si>
+  <si>
+    <t>age 6, bDay after : yes</t>
+  </si>
+  <si>
+    <t>age 6, bDay before : too old</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Multiple returns</t>
+  </si>
+  <si>
+    <t>Web app I functionality</t>
+  </si>
+  <si>
+    <t>Web app II functionality</t>
+  </si>
+  <si>
+    <t>Web app III functionality</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -156,6 +177,13 @@
       <color theme="1"/>
       <name val="Calibri (Body)_x0000_"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -177,11 +205,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,31 +526,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3216228F-B421-8943-9C69-C9FAC1E7C520}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection sqref="A1:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="6" max="6" width="2.5" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -530,17 +562,20 @@
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="G4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2">
         <v>10</v>
@@ -549,135 +584,136 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>2</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5">
+        <v>4</v>
+      </c>
+      <c r="E9" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="D9">
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="5">
+        <v>5</v>
+      </c>
+      <c r="E11" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="5">
         <v>4</v>
       </c>
-      <c r="E9">
+      <c r="E12" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="5">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="2">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="2">
-        <v>5</v>
-      </c>
-      <c r="E11" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>4</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="D14" s="5">
+        <v>6</v>
+      </c>
+      <c r="E14" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="5">
+        <v>6</v>
+      </c>
+      <c r="E15" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="5">
+        <v>2</v>
+      </c>
+      <c r="E16" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D17" s="5">
         <v>6</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E17" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="2">
-        <v>2</v>
-      </c>
-      <c r="E14" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15">
-        <v>6</v>
-      </c>
-      <c r="E15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="2">
-        <v>6</v>
-      </c>
-      <c r="E16" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="2">
-        <v>2</v>
-      </c>
-      <c r="E17" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>7</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="5">
         <v>2</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -690,74 +726,96 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s">
         <v>16</v>
       </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
+      <c r="F25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
         <v>30</v>
       </c>
-      <c r="C23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" t="s">
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
         <v>23</v>
-      </c>
-      <c r="D24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates and new materials
</commit_message>
<xml_diff>
--- a/Labs/Lab03/CS133JS_Lab03_Rubric.xlsx
+++ b/Labs/Lab03/CS133JS_Lab03_Rubric.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS133JS-CourseMaterials/Labs/Lab03/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS133JS-CourseMaterials\Labs\Lab03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95F548B-A2F9-B34E-9AC8-E6D4D0248CF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF184E51-352E-4312-8896-417FF8749C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6560" yWindow="500" windowWidth="15360" windowHeight="14540" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="30948" yWindow="4416" windowWidth="17628" windowHeight="12024" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Group A" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Criteria</t>
   </si>
@@ -90,9 +100,6 @@
     <t>Syntax error in console</t>
   </si>
   <si>
-    <t>Code in the .js file</t>
-  </si>
-  <si>
     <t>Kindergarten Admission, Beverage Labeling, or Trail Difficulty</t>
   </si>
   <si>
@@ -142,6 +149,18 @@
   </si>
   <si>
     <t>Web app III functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trail difficulety: </t>
+  </si>
+  <si>
+    <t>Beverage Labeling:</t>
+  </si>
+  <si>
+    <t>"Fruit juice" : 100% juice, &lt; 4% sweetener, "Fruit Drink" : juice &gt;= 5%, "Fruit flavored drink" : anything</t>
+  </si>
+  <si>
+    <t>Start with the shortest and lowest for process of elimination</t>
   </si>
 </sst>
 </file>
@@ -205,13 +224,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,17 +546,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3216228F-B421-8943-9C69-C9FAC1E7C520}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:G33"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.796875" customWidth="1"/>
     <col min="6" max="6" width="2.5" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -563,7 +583,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -577,12 +597,13 @@
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="5">
         <v>10</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="5">
         <v>10</v>
       </c>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
@@ -604,7 +625,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="5">
         <v>4</v>
@@ -626,7 +647,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D11" s="5">
         <v>5</v>
@@ -637,7 +658,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="5">
         <v>4</v>
@@ -671,7 +692,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="5">
         <v>6</v>
@@ -736,7 +757,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -753,18 +774,18 @@
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="B25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
         <v>16</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -772,54 +793,70 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
         <v>29</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>30</v>
-      </c>
-      <c r="D29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="C30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" t="s">
         <v>32</v>
       </c>
-      <c r="D30" t="s">
-        <v>33</v>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" t="s">
         <v>24</v>
       </c>
-      <c r="B32" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" t="s">
-        <v>23</v>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates for grade change and minor fixes
</commit_message>
<xml_diff>
--- a/Labs/Lab03/CS133JS_Lab03_Rubric.xlsx
+++ b/Labs/Lab03/CS133JS_Lab03_Rubric.xlsx
@@ -1,25 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS133JS-CourseMaterials/labs/Lab03/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS133JS-CourseMaterials\Labs\Lab03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706582FD-8DA2-E749-BB3E-D9FC5E454E79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA944068-1FA5-4AF0-883E-8BEF47F45B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="5200" windowWidth="13680" windowHeight="15520" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="13068" yWindow="4968" windowWidth="17556" windowHeight="11592" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Score" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -221,8 +232,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,13 +554,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3216228F-B421-8943-9C69-C9FAC1E7C520}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D36" sqref="A31:D36"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.796875" customWidth="1"/>
+    <col min="4" max="4" width="8.3984375" customWidth="1"/>
     <col min="6" max="6" width="2.5" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
@@ -584,126 +600,112 @@
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="5">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="G6" s="6"/>
+      <c r="D6">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="5">
-        <v>2</v>
-      </c>
-      <c r="E8" s="5"/>
+      <c r="D8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="5">
-        <v>4</v>
-      </c>
-      <c r="E9" s="5"/>
+      <c r="D9">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="5">
-        <v>5</v>
-      </c>
-      <c r="E11" s="5"/>
+      <c r="D11">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="5">
-        <v>4</v>
-      </c>
-      <c r="E12" s="5"/>
+      <c r="D12">
+        <v>3</v>
+      </c>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="5">
-        <v>2</v>
-      </c>
-      <c r="E13" s="5"/>
+      <c r="D13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="5">
-        <v>6</v>
-      </c>
-      <c r="E14" s="5"/>
+      <c r="D14">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="5">
-        <v>6</v>
-      </c>
-      <c r="E15" s="5"/>
+      <c r="D15">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="5">
-        <v>2</v>
-      </c>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="5">
-        <v>6</v>
-      </c>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="5">
-        <v>2</v>
-      </c>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>3</v>
       </c>
       <c r="D20">
         <f>SUM(D6:D18)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -717,14 +719,16 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
-    <col min="6" max="6" width="2.5" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="3" max="3" width="22.796875" customWidth="1"/>
+    <col min="4" max="4" width="7.69921875" customWidth="1"/>
+    <col min="5" max="5" width="6.19921875" customWidth="1"/>
+    <col min="6" max="6" width="1.796875" customWidth="1"/>
+    <col min="7" max="7" width="16.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -765,13 +769,13 @@
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="5">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5">
-        <v>10</v>
-      </c>
-      <c r="G6" s="6"/>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
@@ -779,143 +783,154 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="5">
-        <v>2</v>
-      </c>
-      <c r="E8" s="5">
-        <v>2</v>
-      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="5">
-        <v>4</v>
-      </c>
-      <c r="E9" s="5">
-        <v>4</v>
-      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10">
         <v>1</v>
       </c>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="5">
-        <v>5</v>
-      </c>
-      <c r="E11" s="5">
-        <v>5</v>
-      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="5">
-        <v>4</v>
-      </c>
-      <c r="E12" s="5">
-        <v>4</v>
-      </c>
-      <c r="G12" s="4"/>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="5">
-        <v>2</v>
-      </c>
-      <c r="E13" s="5">
-        <v>2</v>
-      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="5">
-        <v>6</v>
-      </c>
-      <c r="E14" s="5">
-        <v>6</v>
-      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="5">
-        <v>6</v>
-      </c>
-      <c r="E15" s="5">
-        <v>6</v>
-      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="5">
-        <v>2</v>
-      </c>
-      <c r="E16" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="5">
-        <v>6</v>
-      </c>
-      <c r="E17" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="5">
-        <v>2</v>
-      </c>
-      <c r="E18" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>3</v>
       </c>
       <c r="D20">
         <f>SUM(D6:D18)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E20">
         <f>SUM(E6:E18)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -923,7 +938,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -937,7 +952,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7">
       <c r="B24" t="s">
         <v>20</v>
       </c>
@@ -945,7 +960,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7">
       <c r="B25" t="s">
         <v>27</v>
       </c>
@@ -956,7 +971,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -964,7 +979,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -972,7 +987,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -983,7 +998,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:7">
       <c r="C30" t="s">
         <v>31</v>
       </c>
@@ -991,7 +1006,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -999,7 +1014,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Cosmetic changes to the rubric
</commit_message>
<xml_diff>
--- a/Labs/Lab03/CS133JS_Lab03_Rubric.xlsx
+++ b/Labs/Lab03/CS133JS_Lab03_Rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS133JS-CourseMaterials\Labs\Lab03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS133JS-CourseMaterials/Labs/Lab03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D57C39-A787-45B5-9B2D-A19B3099563E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40FA854-EEA1-C045-9FBE-950DE451D277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="19992" windowHeight="16116" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="24100" yWindow="500" windowWidth="16700" windowHeight="21480" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
     <t>Start with the shortest and lowest for process of elimination</t>
   </si>
   <si>
-    <t>Very good work! Here's the grade breakdown:</t>
+    <t>Very good work on part 1, but you have return statements inside of if statements which is not considered good practice. Excellent work on part 2!  Here's the grade breakdown:</t>
   </si>
 </sst>
 </file>
@@ -241,7 +241,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -564,13 +564,13 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D18"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="22.796875" customWidth="1"/>
-    <col min="4" max="4" width="8.3984375" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
     <col min="6" max="6" width="2.5" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
@@ -728,16 +728,16 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="22.796875" customWidth="1"/>
-    <col min="4" max="4" width="7.69921875" customWidth="1"/>
-    <col min="5" max="5" width="6.19921875" customWidth="1"/>
-    <col min="6" max="6" width="1.796875" customWidth="1"/>
-    <col min="7" max="7" width="16.8984375" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" customWidth="1"/>
+    <col min="6" max="6" width="1.1640625" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -750,7 +750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="36" customHeight="1">
+    <row r="3" spans="1:7" ht="61" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Improved the grading rubric, added ESLint config, updated code reviews for lab 4 and overall style guide
</commit_message>
<xml_diff>
--- a/Labs/Lab03/CS133JS_Lab03_Rubric.xlsx
+++ b/Labs/Lab03/CS133JS_Lab03_Rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS133JS-Repos\CS133JS-CourseMaterials\Labs\Lab03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D506594-99F6-4393-A638-3A3D3380882B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2A7C50-D922-4F72-8668-0811407C93C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22320" yWindow="4236" windowWidth="13800" windowHeight="12960" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="-13980" yWindow="4284" windowWidth="13800" windowHeight="12960" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
   <si>
     <t>Criteria</t>
   </si>
@@ -261,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -283,7 +283,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,10 +761,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAB77B8-CDA3-BE44-A798-E60D57B0DC8A}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -777,17 +776,17 @@
     <col min="7" max="7" width="16.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="32.4" customHeight="1">
+    <row r="3" spans="1:8" ht="32.4" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>50</v>
       </c>
@@ -796,7 +795,7 @@
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="10" t="s">
         <v>39</v>
       </c>
@@ -805,7 +804,7 @@
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>1</v>
@@ -817,15 +816,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="D7">
@@ -837,20 +836,24 @@
       <c r="G7" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="11"/>
+      <c r="H7" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -863,17 +866,22 @@
       <c r="G10" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
       <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -886,8 +894,11 @@
       <c r="G13" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -900,8 +911,11 @@
       <c r="G14" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -914,8 +928,11 @@
       <c r="G15" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -928,17 +945,22 @@
       <c r="G16" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="7" t="s">
         <v>44</v>
       </c>
       <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -951,8 +973,11 @@
       <c r="G19" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -965,8 +990,11 @@
       <c r="G20" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -979,8 +1007,11 @@
       <c r="G21" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -993,17 +1024,22 @@
       <c r="G22" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="7" t="s">
         <v>47</v>
       </c>
       <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -1016,8 +1052,11 @@
       <c r="G25" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1030,8 +1069,11 @@
       <c r="G26" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1044,8 +1086,11 @@
       <c r="G27" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1058,8 +1103,11 @@
       <c r="G28" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1072,8 +1120,11 @@
       <c r="G29" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1086,7 +1137,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>13</v>
       </c>

</xml_diff>